<commit_message>
Completed order function and tested with test code
</commit_message>
<xml_diff>
--- a/Doc/Test Cases.xlsx
+++ b/Doc/Test Cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Case" sheetId="1" r:id="rId1"/>
+    <sheet name="Implement Target" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,69 +16,147 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
   <si>
+    <t>Create Assets</t>
+  </si>
+  <si>
+    <t>Create Programs</t>
+  </si>
+  <si>
+    <t>Create Requests</t>
+  </si>
+  <si>
+    <t>Order Task</t>
+  </si>
+  <si>
+    <t>Assign Assets</t>
+  </si>
+  <si>
+    <t>Serialize and Deserialize</t>
+  </si>
+  <si>
+    <t>Input verification</t>
+  </si>
+  <si>
+    <t>Manully order task</t>
+  </si>
+  <si>
+    <t>Progress Bar</t>
+  </si>
+  <si>
+    <t>Assets pool update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assign chamber to task with no chamber recipe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assign assets which are in use</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only different priority</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only different chamber recipe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Different priority and chamber recipe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Case</t>
-  </si>
-  <si>
-    <t>Create Assets</t>
-  </si>
-  <si>
-    <t>Create Programs</t>
-  </si>
-  <si>
-    <t>Create Requests</t>
-  </si>
-  <si>
-    <t>Order Task</t>
-  </si>
-  <si>
-    <t>Run Task</t>
-  </si>
-  <si>
-    <t>Commit Task Result</t>
-  </si>
-  <si>
-    <t>Assign Assets</t>
-  </si>
-  <si>
-    <t>Update Estimate Duration</t>
-  </si>
-  <si>
-    <t>Update Request Summary</t>
-  </si>
-  <si>
-    <t>Set Result to Invalid</t>
-  </si>
-  <si>
-    <t>Serialize and Deserialize</t>
-  </si>
-  <si>
-    <t>Input verification</t>
-  </si>
-  <si>
-    <t>Manully order task</t>
-  </si>
-  <si>
-    <t>Progress Bar</t>
-  </si>
-  <si>
-    <t>Update Assets Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sub Case</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>One Ready task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Several ready tasks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No ready task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commit running task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commit task which is not running</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commit Task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Execute Task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abandon Task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abandon waiting task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abandon ready task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abandon other type tasks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalidate Task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalidte completed task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalidte running task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Expected Result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -102,19 +180,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -188,6 +274,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -222,6 +309,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -397,172 +485,239 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="B16" t="s">
-        <v>15</v>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C20" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented many test cases
</commit_message>
<xml_diff>
--- a/Doc/Test Cases.xlsx
+++ b/Doc/Test Cases.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -49,10 +48,6 @@
     <t>Progress Bar</t>
   </si>
   <si>
-    <t>Assets pool update</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Assign chamber to task with no chamber recipe</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -93,77 +88,98 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Commit running task</t>
+    <t>Commit Task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Execute Task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abandon Task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalidate Task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Expected Result</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Commit task which is not running</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commit Task</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Execute Task</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Abandon Task</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assign assets when there is no waiting task</t>
+  </si>
+  <si>
+    <t>Commit running task to Complete</t>
+  </si>
+  <si>
+    <t>Commit running task to Invalid</t>
+  </si>
+  <si>
+    <t>Commit running task to other status</t>
   </si>
   <si>
     <t>Abandon waiting task</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Abandon ready task</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Abandon other type tasks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Invalidate Task</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Invalidte completed task</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Invalidte running task</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Expected Result</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Recipe and tester are not compatiable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Recipe and battery model are not compatiable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abandon running task</t>
+  </si>
+  <si>
+    <t>Abandon completed task</t>
+  </si>
+  <si>
+    <t>Abandon invalid task</t>
+  </si>
+  <si>
+    <t>Abandon abandoned task</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
+  <si>
+    <t>Recipe and tester are not compatible</t>
+  </si>
+  <si>
+    <t>Recipe and battery model are not compatible</t>
+  </si>
+  <si>
+    <t>Invalidate completed task</t>
+  </si>
+  <si>
+    <t>Invalidate running task</t>
+  </si>
+  <si>
+    <t>Invalidate task which is not running or completed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -196,7 +212,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -209,7 +225,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -283,7 +299,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -318,7 +333,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -494,61 +508,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -556,20 +583,29 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C6" t="s">
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>5</v>
       </c>
@@ -577,99 +613,194 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="C10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="C11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
         <v>6</v>
       </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="C14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C13" t="s">
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="C15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C14" t="s">
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
       </c>
       <c r="C20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="C21" t="s">
         <v>31</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -680,17 +811,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1">
         <v>12</v>
       </c>
@@ -698,7 +829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>13</v>
       </c>
@@ -706,7 +837,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>14</v>
       </c>
@@ -714,7 +845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -726,13 +857,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>